<commit_message>
impl/storing photo urls in a db
</commit_message>
<xml_diff>
--- a/reports/Отчёт за 18.04.2025.xlsx
+++ b/reports/Отчёт за 18.04.2025.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
   <si>
     <t>Дата</t>
   </si>
@@ -41,19 +41,31 @@
     <t>18.04.2025</t>
   </si>
   <si>
-    <t>АОР</t>
-  </si>
-  <si>
-    <t>пахота зяби</t>
-  </si>
-  <si>
-    <t>многолетние травы</t>
-  </si>
-  <si>
-    <t>предпосевная культура</t>
-  </si>
-  <si>
-    <t>озимая пшеница</t>
+    <t>тск</t>
+  </si>
+  <si>
+    <t>вспашка</t>
+  </si>
+  <si>
+    <t>кукурузу</t>
+  </si>
+  <si>
+    <t>70</t>
+  </si>
+  <si>
+    <t>Не указано</t>
+  </si>
+  <si>
+    <t>100 выравнивание зяби</t>
+  </si>
+  <si>
+    <t>сою</t>
+  </si>
+  <si>
+    <t>155</t>
+  </si>
+  <si>
+    <t>1377</t>
   </si>
 </sst>
 </file>
@@ -157,8 +169,8 @@
   <cols>
     <col min="1" max="1" width="12.5390625" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="22.03125" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="26.74609375" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="22.546875" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="27.22265625" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="13.52734375" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="15.4296875" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="30.78125" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="19.60546875" customWidth="true" bestFit="true"/>
@@ -204,17 +216,17 @@
       <c r="D2" t="s" s="1">
         <v>11</v>
       </c>
-      <c r="E2" t="n" s="1">
-        <v>26.0</v>
-      </c>
-      <c r="F2" t="n" s="1">
-        <v>488.0</v>
-      </c>
-      <c r="G2" t="n" s="1">
-        <v>-1.0</v>
-      </c>
-      <c r="H2" t="n" s="1">
-        <v>-1.0</v>
+      <c r="E2" t="s" s="1">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s" s="1">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s" s="1">
+        <v>13</v>
+      </c>
+      <c r="H2" t="s" s="1">
+        <v>13</v>
       </c>
     </row>
     <row r="3">
@@ -222,25 +234,25 @@
         <v>8</v>
       </c>
       <c r="B3" t="s" s="1">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s" s="1">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D3" t="s" s="1">
-        <v>13</v>
-      </c>
-      <c r="E3" t="n" s="1">
-        <v>215.0</v>
-      </c>
-      <c r="F3" t="n" s="1">
-        <v>1015.0</v>
-      </c>
-      <c r="G3" t="n" s="1">
-        <v>-1.0</v>
-      </c>
-      <c r="H3" t="n" s="1">
-        <v>-1.0</v>
+        <v>15</v>
+      </c>
+      <c r="E3" t="s" s="1">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s" s="1">
+        <v>17</v>
+      </c>
+      <c r="G3" t="s" s="1">
+        <v>13</v>
+      </c>
+      <c r="H3" t="s" s="1">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>